<commit_message>
DB Connection changed,few sleep removed,till HTML
</commit_message>
<xml_diff>
--- a/src/test/resources/Documents/25931/Actual/JobMaterial.xlsx
+++ b/src/test/resources/Documents/25931/Actual/JobMaterial.xlsx
@@ -6,45 +6,100 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Material" r:id="rId3" sheetId="1"/>
+    <sheet name="Planning" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="49">
-  <si>
-    <t>Materialtype</t>
-  </si>
-  <si>
-    <t>Element</t>
-  </si>
-  <si>
-    <t>Process</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Measurementunit</t>
-  </si>
-  <si>
-    <t>Provided</t>
-  </si>
-  <si>
-    <t>Inventoryitem</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="46">
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Planninggroup</t>
+  </si>
+  <si>
+    <t>ScheduledResource</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>PlannedQty</t>
+  </si>
+  <si>
+    <t>Producedqty</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Productionstarted</t>
+  </si>
+  <si>
+    <t>Productionconcluded</t>
   </si>
   <si>
     <t>Plant</t>
   </si>
   <si>
+    <t>ProductionDivision</t>
+  </si>
+  <si>
     <t>MISJobID</t>
   </si>
   <si>
-    <t>1b-Design Jet</t>
+    <t>MISWorkCenter</t>
+  </si>
+  <si>
+    <t>PlannedResource</t>
+  </si>
+  <si>
+    <t>Kit</t>
+  </si>
+  <si>
+    <t>- P-Dinh</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Farmout 1</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>Not allocated</t>
+  </si>
+  <si>
+    <t>- Anderson</t>
+  </si>
+  <si>
+    <t>Farmout 2</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>Liner  2p</t>
+  </si>
+  <si>
+    <t>Cut for Press</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>Cut for Press
+Final Trim</t>
   </si>
   <si>
     <t>Outer wrap  2p</t>
@@ -53,58 +108,40 @@
     <t>Print F 2x0</t>
   </si>
   <si>
-    <t>Design Jet - 19x25</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>Ea</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>445 - iQuote - Proofs - Each</t>
-  </si>
-  <si>
-    <t>Ink / Varnish</t>
-  </si>
-  <si>
-    <t>Black - UV</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>lbs</t>
-  </si>
-  <si>
-    <t>UV-4 CP - UV- 4 Color Process</t>
-  </si>
-  <si>
-    <t>Pantone-1 - UV</t>
-  </si>
-  <si>
-    <t>0.14</t>
-  </si>
-  <si>
-    <t>UV-PMS - UV-PMS</t>
+    <t>8CS 40" (#9)</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>8CS 40" (#9)
+8CP 40" (#9)</t>
+  </si>
+  <si>
+    <t>Laminate</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>Farmout 1
+Farmout 2
+Farmout 3</t>
   </si>
   <si>
     <t>Print F (Varnish 1x0)</t>
   </si>
   <si>
-    <t>SGUV - Cyrel - (Post Finishing)</t>
-  </si>
-  <si>
-    <t>0.27</t>
-  </si>
-  <si>
-    <t>uv - UV coating</t>
-  </si>
-  <si>
-    <t>Plate</t>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Post-Press Cut</t>
+  </si>
+  <si>
+    <t>Final Trim</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
   <si>
     <t>Plate - Outer wrap  2p</t>
@@ -113,52 +150,10 @@
     <t>Plate burn</t>
   </si>
   <si>
-    <t>CTP 40"</t>
-  </si>
-  <si>
-    <t>2.00</t>
-  </si>
-  <si>
-    <t>CTP40 - CTP Plate 40"</t>
-  </si>
-  <si>
-    <t>Cyrel Plate</t>
-  </si>
-  <si>
-    <t>450 - ***40" Cyrel Plate for Press_________***</t>
-  </si>
-  <si>
-    <t>Sheet</t>
-  </si>
-  <si>
-    <t>Liner  2p</t>
-  </si>
-  <si>
-    <t>Cut for Press</t>
-  </si>
-  <si>
-    <t>Special Order Coated Book Non FSC 100 24 x 36" 400 ppi</t>
-  </si>
-  <si>
-    <t>150.00</t>
-  </si>
-  <si>
-    <t>Sht.</t>
-  </si>
-  <si>
-    <t>429 - Offset Stock cost ea for Jobs Only-Use  for shipping too.</t>
-  </si>
-  <si>
-    <t>Sterling Ultra C1S Gloss Verso Non FSC 80# 19 x 25" 500 ppi</t>
-  </si>
-  <si>
-    <t>400.00</t>
-  </si>
-  <si>
-    <t>Sht</t>
-  </si>
-  <si>
-    <t>430 - Offset Stock Per 1000 cost for Jobs Only</t>
+    <t>Galileo</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -166,13 +161,213 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="66">
+  <fonts count="106">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="14.0"/>
+      <color indexed="10"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -520,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -587,6 +782,46 @@
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="68" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="70" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="71" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="74" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="76" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="80" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="82" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="88" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="90" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="92" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="94" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="96" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="98" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="102" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="104" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -630,213 +865,351 @@
       <c r="J1" t="s" s="1">
         <v>9</v>
       </c>
+      <c r="K1" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s" s="1">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s" s="1">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s" s="1">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s" s="5">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s" s="6">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s" s="7">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s" s="8">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s" s="9">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="I2" t="s" s="10">
+        <v>21</v>
+      </c>
+      <c r="J2" t="s" s="11">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s" s="12">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s" s="14">
+        <v>19</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="s" s="10">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s" s="13">
-        <v>19</v>
-      </c>
-      <c r="E3" t="s" s="14">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s" s="15">
+      <c r="A3" t="s" s="15">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s" s="16">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s" s="17">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s" s="18">
+        <v>23</v>
+      </c>
+      <c r="E3" t="s" s="19">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s" s="20">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s" s="21">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s" s="22">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s" s="23">
         <v>21</v>
       </c>
-      <c r="G3" t="s" s="16">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s" s="17">
-        <v>22</v>
+      <c r="J3" t="s" s="24">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s" s="25">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s" s="26">
+        <v>23</v>
+      </c>
+      <c r="M3" t="s" s="27">
+        <v>23</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="18">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s" s="20">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s" s="21">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s" s="22">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s" s="23">
+      <c r="A4" t="s" s="28">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s" s="29">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s" s="30">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s" s="31">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s" s="32">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s" s="33">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s" s="34">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s" s="35">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s" s="36">
         <v>21</v>
       </c>
-      <c r="G4" t="s" s="24">
-        <v>16</v>
-      </c>
-      <c r="H4" t="s" s="25">
-        <v>25</v>
+      <c r="J4" t="s" s="37">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s" s="38">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s" s="39">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s" s="40">
+        <v>28</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="s" s="26">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s" s="27">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s" s="28">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s" s="29">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s" s="30">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s" s="31">
+      <c r="A5" t="s" s="41">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s" s="42">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s" s="43">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s" s="44">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s" s="45">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s" s="46">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s" s="47">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s" s="48">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s" s="49">
         <v>21</v>
       </c>
-      <c r="G5" t="s" s="32">
-        <v>16</v>
-      </c>
-      <c r="H5" t="s" s="33">
-        <v>29</v>
+      <c r="J5" t="s" s="50">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s" s="51">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s" s="52">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s" s="53">
+        <v>33</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="s" s="34">
-        <v>30</v>
-      </c>
-      <c r="B6" t="s" s="35">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s" s="36">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s" s="37">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s" s="38">
+      <c r="A6" t="s" s="54">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s" s="55">
         <v>34</v>
       </c>
-      <c r="F6" t="s" s="39">
-        <v>15</v>
-      </c>
-      <c r="G6" t="s" s="40">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s" s="41">
+      <c r="C6" t="s" s="56">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s" s="57">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s" s="58">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s" s="59">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s" s="60">
         <v>35</v>
+      </c>
+      <c r="H6" t="s" s="61">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s" s="62">
+        <v>21</v>
+      </c>
+      <c r="J6" t="s" s="63">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s" s="64">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s" s="65">
+        <v>19</v>
+      </c>
+      <c r="M6" t="s" s="66">
+        <v>36</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s" s="42">
-        <v>30</v>
-      </c>
-      <c r="B7" t="s" s="43">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s" s="44">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s" s="45">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s" s="46">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s" s="47">
-        <v>15</v>
-      </c>
-      <c r="G7" t="s" s="48">
-        <v>16</v>
-      </c>
-      <c r="H7" t="s" s="49">
+      <c r="A7" t="s" s="67">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s" s="68">
         <v>37</v>
+      </c>
+      <c r="C7" t="s" s="69">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s" s="70">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s" s="71">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s" s="72">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s" s="73">
+        <v>38</v>
+      </c>
+      <c r="H7" t="s" s="74">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s" s="75">
+        <v>21</v>
+      </c>
+      <c r="J7" t="s" s="76">
+        <v>18</v>
+      </c>
+      <c r="K7" t="s" s="77">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s" s="78">
+        <v>31</v>
+      </c>
+      <c r="M7" t="s" s="79">
+        <v>33</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="s" s="50">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s" s="51">
+      <c r="A8" t="s" s="80">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s" s="81">
         <v>39</v>
       </c>
-      <c r="C8" t="s" s="52">
+      <c r="C8" t="s" s="82">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s" s="83">
         <v>40</v>
       </c>
-      <c r="D8" t="s" s="53">
+      <c r="E8" t="s" s="84">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s" s="85">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s" s="86">
         <v>41</v>
       </c>
-      <c r="E8" t="s" s="54">
-        <v>42</v>
-      </c>
-      <c r="F8" t="s" s="55">
-        <v>43</v>
-      </c>
-      <c r="G8" t="s" s="56">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s" s="57">
-        <v>44</v>
+      <c r="H8" t="s" s="87">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s" s="88">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s" s="89">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s" s="90">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s" s="91">
+        <v>40</v>
+      </c>
+      <c r="M8" t="s" s="92">
+        <v>28</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="s" s="58">
-        <v>38</v>
-      </c>
-      <c r="B9" t="s" s="59">
-        <v>11</v>
-      </c>
-      <c r="C9" t="s" s="60">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s" s="61">
+      <c r="A9" t="s" s="93">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s" s="94">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s" s="95">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s" s="96">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s" s="97">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s" s="98">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s" s="99">
         <v>45</v>
       </c>
-      <c r="E9" t="s" s="62">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s" s="63">
-        <v>47</v>
-      </c>
-      <c r="G9" t="s" s="64">
-        <v>16</v>
-      </c>
-      <c r="H9" t="s" s="65">
-        <v>48</v>
+      <c r="H9" t="s" s="100">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s" s="101">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s" s="102">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s" s="103">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s" s="104">
+        <v>44</v>
+      </c>
+      <c r="M9" t="s" s="105">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>